<commit_message>
added set_colors function for dynamic line color plotting
</commit_message>
<xml_diff>
--- a/geologic/input/Template_Well_Data.xlsx
+++ b/geologic/input/Template_Well_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhodges/projects/hydrogeo_plots/geologic/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50242940-D725-0C47-AFCE-838D26D4EAF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB1DA78-D89B-E04E-9C2C-FF1610280C97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="805" activeTab="2" xr2:uid="{6DE61712-4CD2-48F1-B856-0F76BADD48E1}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="805" activeTab="4" xr2:uid="{6DE61712-4CD2-48F1-B856-0F76BADD48E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Lithology_Elev" sheetId="25" r:id="rId1"/>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="148">
   <si>
     <t>Depth_Top_ft</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Material</t>
   </si>
   <si>
-    <t>screen</t>
-  </si>
-  <si>
     <t>Depth_ft</t>
   </si>
   <si>
@@ -456,9 +453,6 @@
     <t>230-261 []</t>
   </si>
   <si>
-    <t>casing</t>
-  </si>
-  <si>
     <t>sanitary seal</t>
   </si>
   <si>
@@ -525,9 +519,6 @@
     <t>ug/L</t>
   </si>
   <si>
-    <t>fill</t>
-  </si>
-  <si>
     <t>TDS_mg/L</t>
   </si>
   <si>
@@ -550,6 +541,27 @@
   </si>
   <si>
     <t>five</t>
+  </si>
+  <si>
+    <t>SDLD6</t>
+  </si>
+  <si>
+    <t>SDLD5</t>
+  </si>
+  <si>
+    <t>SDLD4</t>
+  </si>
+  <si>
+    <t>SDLD3</t>
+  </si>
+  <si>
+    <t>SDLD2</t>
+  </si>
+  <si>
+    <t>SDLD1</t>
+  </si>
+  <si>
+    <t>well_id</t>
   </si>
 </sst>
 </file>
@@ -2141,19 +2153,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>96</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>97</v>
       </c>
       <c r="G1" s="24">
         <v>90</v>
@@ -2167,7 +2179,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D2" s="24">
         <f t="shared" ref="D2:D20" si="0">$G$1-A2</f>
@@ -2187,7 +2199,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" s="24">
         <f t="shared" si="0"/>
@@ -2207,7 +2219,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" s="24">
         <f t="shared" si="0"/>
@@ -2227,7 +2239,7 @@
         <v>30</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" s="24">
         <f t="shared" si="0"/>
@@ -2247,7 +2259,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="24">
         <f t="shared" si="0"/>
@@ -2267,7 +2279,7 @@
         <v>67</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="24">
         <f t="shared" si="0"/>
@@ -2287,7 +2299,7 @@
         <v>93</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" s="24">
         <f t="shared" si="0"/>
@@ -2307,7 +2319,7 @@
         <v>103</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D9" s="24">
         <f t="shared" si="0"/>
@@ -2327,7 +2339,7 @@
         <v>128</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10" s="24">
         <f t="shared" si="0"/>
@@ -2347,7 +2359,7 @@
         <v>144</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D11" s="24">
         <f t="shared" si="0"/>
@@ -2367,7 +2379,7 @@
         <v>201</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D12" s="24">
         <f t="shared" si="0"/>
@@ -2387,7 +2399,7 @@
         <v>260</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" s="24">
         <f t="shared" si="0"/>
@@ -2407,7 +2419,7 @@
         <v>273</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D14" s="24">
         <f t="shared" si="0"/>
@@ -2427,7 +2439,7 @@
         <v>346</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="24">
         <f t="shared" si="0"/>
@@ -2447,7 +2459,7 @@
         <v>444</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="24">
         <f t="shared" si="0"/>
@@ -2467,7 +2479,7 @@
         <v>495</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" s="24">
         <f t="shared" si="0"/>
@@ -2487,7 +2499,7 @@
         <v>505</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D18" s="24">
         <f t="shared" si="0"/>
@@ -2507,7 +2519,7 @@
         <v>518</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D19" s="24">
         <f t="shared" si="0"/>
@@ -2527,7 +2539,7 @@
         <v>660</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" s="24">
         <f t="shared" si="0"/>
@@ -2563,19 +2575,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="133" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="132" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="132" t="s">
+      <c r="E1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3666,16 +3678,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="133" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3922,31 +3934,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="126" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="42" t="s">
         <v>71</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" s="42" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4404,31 +4416,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="15" t="s">
         <v>71</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4758,34 +4770,34 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="140" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="140" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G1" t="s">
-        <v>122</v>
-      </c>
       <c r="H1" s="140" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I1"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="24">
         <v>1</v>
@@ -4812,7 +4824,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="24">
         <v>1</v>
@@ -4839,7 +4851,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="24">
         <v>2</v>
@@ -4866,7 +4878,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="24">
         <v>3</v>
@@ -4893,7 +4905,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="24">
         <v>4</v>
@@ -4920,7 +4932,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="24">
         <v>5</v>
@@ -4975,33 +4987,33 @@
   <sheetData>
     <row r="1" spans="1:8" s="24" customFormat="1">
       <c r="A1" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="F1" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>122</v>
-      </c>
       <c r="H1" s="24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="24">
         <v>1</v>
@@ -5018,7 +5030,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="24">
         <v>1</v>
@@ -5033,12 +5045,12 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="24">
         <v>2</v>
@@ -5053,12 +5065,12 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="24">
         <v>3</v>
@@ -5073,12 +5085,12 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="24">
         <v>4</v>
@@ -5093,12 +5105,12 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="24">
         <v>5</v>
@@ -5113,7 +5125,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -5191,54 +5203,54 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="59" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="130" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="130" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="130" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" s="130" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F1" s="130" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="136" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="136" t="s">
-        <v>69</v>
-      </c>
       <c r="H1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="I1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="N1" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="K1" t="s">
-        <v>132</v>
-      </c>
-      <c r="L1" s="59" t="s">
-        <v>125</v>
-      </c>
-      <c r="M1" s="59" t="s">
-        <v>88</v>
-      </c>
-      <c r="N1" s="24" t="s">
-        <v>126</v>
-      </c>
       <c r="O1" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="24" customFormat="1">
       <c r="A2" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="20">
         <v>0</v>
@@ -5290,7 +5302,7 @@
     </row>
     <row r="3" spans="1:19" s="24" customFormat="1">
       <c r="A3" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="20">
         <v>370</v>
@@ -5342,7 +5354,7 @@
     </row>
     <row r="4" spans="1:19" s="24" customFormat="1">
       <c r="A4" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="24">
         <v>380</v>
@@ -5394,7 +5406,7 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="24">
         <v>390</v>
@@ -5446,7 +5458,7 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="24">
         <v>410</v>
@@ -5498,7 +5510,7 @@
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="24">
         <v>430</v>
@@ -5550,7 +5562,7 @@
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="24">
         <v>440</v>
@@ -5602,7 +5614,7 @@
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="24">
         <v>515</v>
@@ -5732,54 +5744,54 @@
   <sheetData>
     <row r="1" spans="1:15" s="24" customFormat="1">
       <c r="A1" s="59" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="130" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="130" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="130" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" s="130" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F1" s="130" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="136" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="136" t="s">
-        <v>69</v>
-      </c>
       <c r="H1" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="I1" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" s="24" t="s">
+      <c r="M1" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="N1" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="K1" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="L1" s="59" t="s">
-        <v>125</v>
-      </c>
-      <c r="M1" s="59" t="s">
-        <v>88</v>
-      </c>
-      <c r="N1" s="24" t="s">
-        <v>126</v>
-      </c>
       <c r="O1" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="24" customFormat="1">
       <c r="A2" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="20">
         <v>0</v>
@@ -5799,7 +5811,7 @@
     </row>
     <row r="3" spans="1:15" s="24" customFormat="1">
       <c r="A3" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="20">
         <v>370</v>
@@ -5819,7 +5831,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="24">
         <v>380</v>
@@ -5842,7 +5854,7 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="24">
         <v>390</v>
@@ -5860,17 +5872,17 @@
       <c r="I5" s="50"/>
       <c r="J5" s="51"/>
       <c r="K5" s="24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="L5" s="24"/>
       <c r="M5" s="24"/>
       <c r="O5" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="24">
         <v>410</v>
@@ -5885,33 +5897,33 @@
       <c r="F6" s="29"/>
       <c r="G6" s="30"/>
       <c r="H6" s="141" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I6" s="141" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="J6" s="141" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="L6" s="141" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="M6" s="141" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="N6" s="141" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="24">
         <v>430</v>
@@ -5929,17 +5941,17 @@
       <c r="I7" s="50"/>
       <c r="J7" s="51"/>
       <c r="K7" s="24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="L7" s="24"/>
       <c r="M7" s="24"/>
       <c r="O7" s="12" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="24">
         <v>440</v>
@@ -5957,17 +5969,17 @@
       <c r="I8" s="49"/>
       <c r="J8" s="51"/>
       <c r="K8" s="24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="L8" s="24"/>
       <c r="M8" s="24"/>
       <c r="O8" s="12" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="24">
         <v>515</v>
@@ -5985,12 +5997,12 @@
       <c r="I9" s="50"/>
       <c r="J9" s="51"/>
       <c r="K9" s="24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="L9" s="24"/>
       <c r="M9" s="24"/>
       <c r="O9" s="12" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -6030,48 +6042,48 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="59" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="130" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="130" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="130" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" s="130" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F1" s="130" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="131" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="131" t="s">
-        <v>69</v>
-      </c>
       <c r="H1" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="K1" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="I1" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" s="24" t="s">
+      <c r="L1" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" s="24" t="s">
         <v>124</v>
-      </c>
-      <c r="K1" s="59" t="s">
-        <v>125</v>
-      </c>
-      <c r="L1" s="59" t="s">
-        <v>88</v>
-      </c>
-      <c r="M1" s="24" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="24">
         <v>0</v>
@@ -6117,7 +6129,7 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="24">
         <v>230</v>
@@ -6164,7 +6176,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="24">
         <f>C3</f>
@@ -6211,7 +6223,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="24">
         <f t="shared" ref="B5:B10" si="5">C4</f>
@@ -6258,7 +6270,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="24">
         <f t="shared" si="5"/>
@@ -6305,7 +6317,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="24">
         <f t="shared" si="5"/>
@@ -6352,7 +6364,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="24">
         <f t="shared" si="5"/>
@@ -6399,7 +6411,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="24">
         <f t="shared" si="5"/>
@@ -6446,7 +6458,7 @@
     </row>
     <row r="10" spans="1:14" ht="16" thickBot="1">
       <c r="A10" s="61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="61">
         <f t="shared" si="5"/>
@@ -6493,7 +6505,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B11" s="20">
         <f>B3</f>
@@ -6541,12 +6553,12 @@
         <v>0.50687873607286638</v>
       </c>
       <c r="N11" s="56" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B12" s="20">
         <f>B7</f>
@@ -6594,12 +6606,12 @@
         <v>3.5643403569837301E-4</v>
       </c>
       <c r="N12" s="56" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="16" thickBot="1">
       <c r="A13" s="64" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B13" s="64">
         <f>B8</f>
@@ -6647,12 +6659,12 @@
         <v>0.49276482989143511</v>
       </c>
       <c r="N13" s="66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="17" thickTop="1" thickBot="1">
       <c r="A14" s="67" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B14" s="68"/>
       <c r="C14" s="68"/>
@@ -6697,7 +6709,7 @@
     </row>
     <row r="15" spans="1:14" ht="16" thickTop="1">
       <c r="A15" s="71" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B15" s="72">
         <f>B13</f>
@@ -6751,7 +6763,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="20"/>
@@ -6772,7 +6784,7 @@
     </row>
     <row r="17" spans="1:14" ht="16" thickBot="1">
       <c r="A17" s="76" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B17" s="77"/>
       <c r="C17" s="77"/>
@@ -6878,42 +6890,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="11">
@@ -6922,10 +6934,10 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="11">
         <v>0.05</v>
@@ -6933,10 +6945,10 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G4" s="10">
         <v>1</v>
@@ -6944,10 +6956,10 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5" s="10">
         <v>10</v>
@@ -6955,10 +6967,10 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="11">
         <v>0.3</v>
@@ -6966,18 +6978,18 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="24" customFormat="1">
       <c r="A8" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="24">
         <v>2.5</v>
@@ -6994,10 +7006,10 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="11">
         <v>2.5</v>
@@ -7014,10 +7026,10 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="11">
         <v>2.5</v>
@@ -7034,10 +7046,10 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="11">
         <v>0.05</v>
@@ -7045,10 +7057,10 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="11">
         <v>0.02</v>
@@ -7059,10 +7071,10 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13">
         <v>2E-3</v>
@@ -7073,10 +7085,10 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="11">
         <v>0.01</v>
@@ -7084,10 +7096,10 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="11">
         <v>10</v>
@@ -7104,18 +7116,18 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="C17" s="11">
         <v>0.1</v>
@@ -7126,10 +7138,10 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="11">
         <v>2.5000000000000001E-2</v>
@@ -7137,10 +7149,10 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -7154,10 +7166,10 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -7171,10 +7183,10 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C21" s="24">
         <v>2</v>
@@ -7220,25 +7232,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="54" t="s">
-        <v>102</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>97</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>98</v>
-      </c>
-      <c r="H1" t="s">
-        <v>99</v>
       </c>
       <c r="I1">
         <v>148</v>
@@ -7264,13 +7276,13 @@
         <v>45</v>
       </c>
       <c r="F2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" t="s">
         <v>99</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>100</v>
-      </c>
-      <c r="H2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -7293,7 +7305,7 @@
         <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -7316,7 +7328,7 @@
         <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -7340,7 +7352,7 @@
         <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -7363,7 +7375,7 @@
         <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -7386,7 +7398,7 @@
         <v>100</v>
       </c>
       <c r="F7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -7409,7 +7421,7 @@
         <v>250</v>
       </c>
       <c r="F8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -7433,114 +7445,114 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
         <v>43</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -7576,48 +7588,48 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="H1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="K1" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="M1" s="24" t="s">
         <v>89</v>
-      </c>
-      <c r="M1" s="24" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="24">
         <v>0</v>
@@ -7662,7 +7674,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="24">
         <v>230</v>
@@ -7708,7 +7720,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="24">
         <f>C3</f>
@@ -7754,7 +7766,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="24">
         <f t="shared" ref="B5:B10" si="4">C4</f>
@@ -7800,7 +7812,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="24">
         <f t="shared" si="4"/>
@@ -7846,7 +7858,7 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="24">
         <f t="shared" si="4"/>
@@ -7892,7 +7904,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="24">
         <f t="shared" si="4"/>
@@ -7938,7 +7950,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="24">
         <f t="shared" si="4"/>
@@ -7984,7 +7996,7 @@
     </row>
     <row r="10" spans="1:13" ht="16" thickBot="1">
       <c r="A10" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="24">
         <f t="shared" si="4"/>
@@ -8075,48 +8087,48 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="H1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="K1" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="M1" s="24" t="s">
         <v>89</v>
-      </c>
-      <c r="M1" s="24" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="43">
         <v>0</v>
@@ -8148,7 +8160,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="24">
         <v>230</v>
@@ -8161,13 +8173,13 @@
         <v>31</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H3" s="47"/>
       <c r="I3" s="47"/>
@@ -8187,7 +8199,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="24">
         <f>C3</f>
@@ -8204,13 +8216,13 @@
       <c r="F4" s="29"/>
       <c r="G4" s="30"/>
       <c r="H4" s="49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I4" s="50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J4" s="51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K4" s="24" t="str">
         <f t="shared" si="1"/>
@@ -8227,7 +8239,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="24">
         <f t="shared" ref="B5:B10" si="3">C4</f>
@@ -8246,7 +8258,7 @@
       <c r="H5" s="50"/>
       <c r="I5" s="49"/>
       <c r="J5" s="51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K5" s="24" t="str">
         <f t="shared" si="1"/>
@@ -8263,7 +8275,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="24">
         <f t="shared" si="3"/>
@@ -8277,20 +8289,20 @@
         <v>30</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G6" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H6" s="49"/>
       <c r="I6" s="50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J6" s="51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K6" s="24" t="str">
         <f t="shared" si="1"/>
@@ -8307,7 +8319,7 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="24">
         <f t="shared" si="3"/>
@@ -8321,20 +8333,20 @@
         <v>80</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H7" s="49"/>
       <c r="I7" s="49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J7" s="51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K7" s="24" t="str">
         <f t="shared" si="1"/>
@@ -8351,7 +8363,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="24">
         <f t="shared" si="3"/>
@@ -8385,7 +8397,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="24">
         <f t="shared" si="3"/>
@@ -8403,10 +8415,10 @@
       <c r="G9" s="33"/>
       <c r="H9" s="50"/>
       <c r="I9" s="50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J9" s="51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K9" s="24" t="str">
         <f t="shared" si="1"/>
@@ -8423,7 +8435,7 @@
     </row>
     <row r="10" spans="1:13" ht="16" thickBot="1">
       <c r="A10" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="24">
         <f t="shared" si="3"/>
@@ -8441,10 +8453,10 @@
       <c r="G10" s="35"/>
       <c r="H10" s="52"/>
       <c r="I10" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J10" s="53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K10" s="24" t="str">
         <f t="shared" si="1"/>
@@ -8472,7 +8484,7 @@
   </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -8489,10 +8501,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -8510,7 +8522,7 @@
         <v>180</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -8526,7 +8538,7 @@
         <v>620</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8542,7 +8554,7 @@
         <v>520</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -8558,7 +8570,7 @@
         <v>980</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -8574,7 +8586,7 @@
         <v>320</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" s="24" customFormat="1"/>
@@ -8610,13 +8622,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -8636,7 +8648,7 @@
         <v>34</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -8654,7 +8666,7 @@
         <v>32</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -8672,7 +8684,7 @@
         <v>30</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -8685,10 +8697,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8705,24 +8717,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="24">
-        <v>0</v>
+        <v>42.5</v>
       </c>
       <c r="B2" s="24">
-        <v>370</v>
+        <v>47.5</v>
       </c>
       <c r="C2" s="24">
         <v>20</v>
@@ -8732,16 +8744,15 @@
         <v>20</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="24">
-        <f>B2</f>
-        <v>370</v>
+        <v>180</v>
       </c>
       <c r="B3" s="24">
-        <v>410</v>
+        <v>200</v>
       </c>
       <c r="C3" s="24">
         <f>D2</f>
@@ -8751,16 +8762,15 @@
         <v>20</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>2</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="24">
-        <f>B3</f>
-        <v>410</v>
+        <v>620</v>
       </c>
       <c r="B4" s="24">
-        <v>430</v>
+        <v>640</v>
       </c>
       <c r="C4" s="24">
         <v>20</v>
@@ -8770,16 +8780,15 @@
         <v>20</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="24">
-        <f>B4</f>
-        <v>430</v>
+        <v>1110</v>
       </c>
       <c r="B5" s="24">
-        <v>540</v>
+        <v>1130</v>
       </c>
       <c r="C5" s="24">
         <f t="shared" ref="C5" si="0">D4</f>
@@ -8790,16 +8799,15 @@
         <v>20</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>2</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="24">
-        <f>B5</f>
-        <v>540</v>
+        <v>2180</v>
       </c>
       <c r="B6" s="24">
-        <v>560</v>
+        <v>2200</v>
       </c>
       <c r="C6" s="24">
         <v>20</v>
@@ -8808,15 +8816,15 @@
         <v>20</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>112</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="24">
-        <v>560</v>
+        <v>2580</v>
       </c>
       <c r="B7" s="24">
-        <v>585</v>
+        <v>2620</v>
       </c>
       <c r="C7" s="24">
         <v>20</v>
@@ -8825,27 +8833,11 @@
         <v>20</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="24">
-        <v>585</v>
-      </c>
-      <c r="B8" s="24">
-        <v>678</v>
-      </c>
-      <c r="C8" s="24">
-        <v>17.5</v>
-      </c>
-      <c r="D8" s="24">
-        <v>17.5</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8875,13 +8867,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>1</v>
@@ -8917,13 +8909,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -8959,13 +8951,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -8986,7 +8978,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -9005,7 +8997,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="24" customFormat="1">
@@ -9024,7 +9016,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -9050,10 +9042,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -9061,7 +9053,7 @@
         <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -9069,7 +9061,7 @@
         <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>